<commit_message>
PCB and Schematics Update
</commit_message>
<xml_diff>
--- a/Hardware/BikerBlinkerRev1/Project Outputs for BikerBlinkerRev1/BikerBlinkerRev1.xlsx
+++ b/Hardware/BikerBlinkerRev1/Project Outputs for BikerBlinkerRev1/BikerBlinkerRev1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan Moed\Documents\GitHub\BikerBlinker\Hardware\BikerBlinkerRev1\Project Outputs for BikerBlinkerRev1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635652C7-CD91-4572-B6E7-B8C09DE32095}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE3546D-8602-4B8C-9AD4-05A943E83504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="25396" windowHeight="15945" xr2:uid="{57ABF62D-98BD-456F-8C56-B0C7657E032F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="25396" windowHeight="15945" xr2:uid="{09409623-5AEA-4D7F-A4D4-44022EAEE159}"/>
   </bookViews>
   <sheets>
     <sheet name="BikerBlinkerRev1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="105">
   <si>
     <t>Comment</t>
   </si>
@@ -62,7 +62,7 @@
     <t>CAP CER 22UF 6.3V X5R 0603</t>
   </si>
   <si>
-    <t>C1</t>
+    <t>C1, C4, C7, C13</t>
   </si>
   <si>
     <t>SMD-0603C</t>
@@ -95,18 +95,6 @@
     <t>GCM1885C1H100FA16D</t>
   </si>
   <si>
-    <t>68uF</t>
-  </si>
-  <si>
-    <t>CAP CER 0.68UF 10V X7R 0603</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>GRM188R71A684KA61D</t>
-  </si>
-  <si>
     <t>1µF</t>
   </si>
   <si>
@@ -191,18 +179,27 @@
     <t>B2B-PH-K-S(LF)(SN)</t>
   </si>
   <si>
-    <t>Yellow</t>
-  </si>
-  <si>
-    <t>J4, J6</t>
-  </si>
-  <si>
-    <t>Red</t>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>Center</t>
   </si>
   <si>
     <t>J5</t>
   </si>
   <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>1uH</t>
+  </si>
+  <si>
     <t>Inductor</t>
   </si>
   <si>
@@ -212,16 +209,19 @@
     <t>0603</t>
   </si>
   <si>
-    <t>MOSFET-N</t>
-  </si>
-  <si>
-    <t>N-Channel MOSFET</t>
+    <t>2N7002W</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 60V 115MA SOT-323</t>
   </si>
   <si>
     <t>Q1, Q2, Q3</t>
   </si>
   <si>
-    <t>E3</t>
+    <t>FP-419AB-01-IPC_C</t>
+  </si>
+  <si>
+    <t>CMP-07173-000098-1</t>
   </si>
   <si>
     <t>1M</t>
@@ -257,6 +257,9 @@
     <t>R6, R7</t>
   </si>
   <si>
+    <t>2k</t>
+  </si>
+  <si>
     <t>R8</t>
   </si>
   <si>
@@ -311,6 +314,9 @@
     <t>TPS63061DSCR</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>U2</t>
   </si>
   <si>
@@ -345,9 +351,6 @@
   </si>
   <si>
     <t>AP2112K-1.8TRG1</t>
-  </si>
-  <si>
-    <t>5V Buck Boost Converter</t>
   </si>
 </sst>
 </file>
@@ -363,18 +366,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD3D3D3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -386,15 +383,9 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -404,18 +395,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -729,629 +711,624 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CE261B-91AA-4E49-93CD-E6F26E114711}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E42D0B-976B-4C79-BC29-318FCAFDC16D}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.53125" customWidth="1"/>
-    <col min="2" max="2" width="123.06640625" customWidth="1"/>
-    <col min="3" max="3" width="18.53125" customWidth="1"/>
-    <col min="4" max="4" width="33.59765625" customWidth="1"/>
-    <col min="5" max="5" width="22.59765625" customWidth="1"/>
-    <col min="6" max="6" width="18.53125" customWidth="1"/>
+    <col min="1" max="6" width="18.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4">
-        <v>1</v>
+      <c r="F2">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="4">
-        <v>1</v>
+      <c r="F5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1</v>
-      </c>
-    </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="4">
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="3" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="3" t="s">
+      <c r="E12" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="4">
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="4">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="4">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="3" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E24" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="C25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E25" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F24" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25" s="4">
+      <c r="F25">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="A26" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="B26" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="C26" t="s">
         <v>85</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F26" s="4">
+      <c r="D26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="A27" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="B27" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="C27" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F27" s="4">
+      <c r="D27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F28" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F29" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="F30" s="4">
+      <c r="E30" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="65" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
+  <pageSetup scale="62" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>